<commit_message>
Notes Meeting Daniel Tomorrow
File mit die Punkte die wir morgen mit Daniel besprechen sollen. zu
finden in: S.A.W.Z.E\SAWZE_Documentation\Milestone_02
auch paar kleine ergänzungen in Priority plan
</commit_message>
<xml_diff>
--- a/SAWZE_Documentation/Last Mile/SAWZE_priority_plan.xlsx
+++ b/SAWZE_Documentation/Last Mile/SAWZE_priority_plan.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tabelle2!$A$1:$G$81</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tabelle2!$A$1:$G$84</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="149">
   <si>
     <t>Gameplay</t>
   </si>
@@ -442,6 +442,30 @@
   </si>
   <si>
     <t>document and communicate sound and SFX list (with team and Markus)</t>
+  </si>
+  <si>
+    <t>Click menu</t>
+  </si>
+  <si>
+    <t>Sound for "Click" on buttons for menu elements</t>
+  </si>
+  <si>
+    <t>Z-Virus-Cloud</t>
+  </si>
+  <si>
+    <t>kleiner scalieren, damit er sich gehnau auf einem Tile befindet und nicht rüber geht</t>
+  </si>
+  <si>
+    <t>Farben eventuel anpassen um besser auf dem Level zu sichten</t>
+  </si>
+  <si>
+    <t>TS_Opa</t>
+  </si>
+  <si>
+    <t>Out of cloud damage</t>
+  </si>
+  <si>
+    <t>balancing of Healt loss out of the cloud</t>
   </si>
 </sst>
 </file>
@@ -1102,11 +1126,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G81"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:G85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F85" sqref="F85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1116,7 +1141,7 @@
     <col min="3" max="3" width="8.140625" style="12" customWidth="1"/>
     <col min="4" max="4" width="6.28515625" style="4" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" style="4"/>
-    <col min="6" max="6" width="69" style="4" customWidth="1"/>
+    <col min="6" max="6" width="81.42578125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -1142,7 +1167,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>109</v>
       </c>
@@ -1193,7 +1218,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
@@ -1211,7 +1236,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
@@ -1229,7 +1254,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>2</v>
       </c>
@@ -1247,7 +1272,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>2</v>
       </c>
@@ -1265,7 +1290,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>2</v>
       </c>
@@ -1283,7 +1308,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>2</v>
       </c>
@@ -1301,7 +1326,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>2</v>
       </c>
@@ -1319,7 +1344,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>2</v>
       </c>
@@ -1337,7 +1362,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>2</v>
       </c>
@@ -1358,7 +1383,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>2</v>
       </c>
@@ -1376,7 +1401,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>2</v>
       </c>
@@ -1397,7 +1422,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>2</v>
       </c>
@@ -1415,7 +1440,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>2</v>
       </c>
@@ -1436,7 +1461,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>2</v>
       </c>
@@ -1454,7 +1479,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>2</v>
       </c>
@@ -1475,7 +1500,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>0</v>
       </c>
@@ -1493,7 +1518,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>0</v>
       </c>
@@ -1514,7 +1539,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>50</v>
       </c>
@@ -1532,7 +1557,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>50</v>
       </c>
@@ -1553,7 +1578,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>50</v>
       </c>
@@ -1572,7 +1597,7 @@
       </c>
       <c r="G24" s="6"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>50</v>
       </c>
@@ -1590,7 +1615,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>50</v>
       </c>
@@ -1609,7 +1634,7 @@
       </c>
       <c r="G26" s="6"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>50</v>
       </c>
@@ -1627,7 +1652,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>50</v>
       </c>
@@ -1645,7 +1670,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>50</v>
       </c>
@@ -1663,7 +1688,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>50</v>
       </c>
@@ -1681,7 +1706,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>50</v>
       </c>
@@ -1699,7 +1724,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>50</v>
       </c>
@@ -1717,7 +1742,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>50</v>
       </c>
@@ -1735,7 +1760,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>50</v>
       </c>
@@ -1753,7 +1778,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>50</v>
       </c>
@@ -1771,7 +1796,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>70</v>
       </c>
@@ -1789,7 +1814,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>70</v>
       </c>
@@ -1807,7 +1832,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>70</v>
       </c>
@@ -1828,7 +1853,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>70</v>
       </c>
@@ -1846,7 +1871,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>70</v>
       </c>
@@ -1864,7 +1889,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>70</v>
       </c>
@@ -1885,7 +1910,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>7</v>
       </c>
@@ -1963,7 +1988,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>7</v>
       </c>
@@ -1981,7 +2006,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>7</v>
       </c>
@@ -1996,7 +2021,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>7</v>
       </c>
@@ -2011,7 +2036,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>113</v>
       </c>
@@ -2029,7 +2054,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>113</v>
       </c>
@@ -2050,7 +2075,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>113</v>
       </c>
@@ -2068,7 +2093,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>113</v>
       </c>
@@ -2086,7 +2111,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>113</v>
       </c>
@@ -2104,7 +2129,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>113</v>
       </c>
@@ -2122,7 +2147,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>61</v>
       </c>
@@ -2140,7 +2165,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>61</v>
       </c>
@@ -2158,7 +2183,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>61</v>
       </c>
@@ -2176,7 +2201,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>61</v>
       </c>
@@ -2194,7 +2219,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>61</v>
       </c>
@@ -2212,7 +2237,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>61</v>
       </c>
@@ -2230,7 +2255,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>61</v>
       </c>
@@ -2248,7 +2273,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>61</v>
       </c>
@@ -2266,7 +2291,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>61</v>
       </c>
@@ -2284,7 +2309,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>61</v>
       </c>
@@ -2302,7 +2327,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>61</v>
       </c>
@@ -2320,7 +2345,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>61</v>
       </c>
@@ -2338,7 +2363,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>61</v>
       </c>
@@ -2359,7 +2384,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>77</v>
       </c>
@@ -2377,7 +2402,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>77</v>
       </c>
@@ -2395,7 +2420,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>77</v>
       </c>
@@ -2413,7 +2438,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>77</v>
       </c>
@@ -2431,7 +2456,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>77</v>
       </c>
@@ -2449,7 +2474,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>77</v>
       </c>
@@ -2467,7 +2492,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>77</v>
       </c>
@@ -2482,7 +2507,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>77</v>
       </c>
@@ -2497,7 +2522,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>7</v>
       </c>
@@ -2563,7 +2588,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>0</v>
       </c>
@@ -2581,8 +2606,89 @@
         <v>140</v>
       </c>
     </row>
+    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C82" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D82" s="5"/>
+      <c r="E82" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="G82" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C83" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D83" s="5"/>
+      <c r="E83" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F83" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C84" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D84" s="5"/>
+      <c r="E84" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F84" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C85" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D85" s="5"/>
+      <c r="E85" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F85" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G81"/>
+  <autoFilter ref="A1:G84">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Toma"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
level n light n stuff
</commit_message>
<xml_diff>
--- a/SAWZE_Documentation/Last Mile/SAWZE_priority_plan.xlsx
+++ b/SAWZE_Documentation/Last Mile/SAWZE_priority_plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="21315" windowHeight="10035" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="21315" windowHeight="9975" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tabelle2!$A$1:$G$84</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tabelle2!$A$1:$G$85</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -1130,7 +1130,7 @@
   <dimension ref="A1:G85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F85" sqref="F85"/>
     </sheetView>
   </sheetViews>
@@ -1185,7 +1185,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>109</v>
       </c>
@@ -1200,7 +1200,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>109</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
@@ -1254,7 +1254,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>2</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>2</v>
       </c>
@@ -1344,7 +1344,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>2</v>
       </c>
@@ -1362,7 +1362,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>2</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>2</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>2</v>
       </c>
@@ -1440,7 +1440,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>2</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>0</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>0</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>50</v>
       </c>
@@ -1634,7 +1634,7 @@
       </c>
       <c r="G26" s="6"/>
     </row>
-    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>50</v>
       </c>
@@ -1688,7 +1688,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>50</v>
       </c>
@@ -1814,7 +1814,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>70</v>
       </c>
@@ -1832,7 +1832,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>70</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>70</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>70</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>7</v>
       </c>
@@ -1943,7 +1943,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>7</v>
       </c>
@@ -1958,7 +1958,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>7</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>7</v>
       </c>
@@ -2036,7 +2036,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>113</v>
       </c>
@@ -2054,7 +2054,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>113</v>
       </c>
@@ -2075,7 +2075,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>113</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>113</v>
       </c>
@@ -2165,7 +2165,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>61</v>
       </c>
@@ -2201,7 +2201,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>61</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>61</v>
       </c>
@@ -2273,7 +2273,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>61</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>61</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>61</v>
       </c>
@@ -2363,7 +2363,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>61</v>
       </c>
@@ -2456,7 +2456,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>77</v>
       </c>
@@ -2522,7 +2522,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>7</v>
       </c>
@@ -2540,7 +2540,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>109</v>
       </c>
@@ -2555,7 +2555,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>109</v>
       </c>
@@ -2573,7 +2573,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>109</v>
       </c>
@@ -2588,7 +2588,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>0</v>
       </c>
@@ -2606,7 +2606,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>113</v>
       </c>
@@ -2627,7 +2627,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>0</v>
       </c>
@@ -2663,7 +2663,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>0</v>
       </c>
@@ -2682,10 +2682,10 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G84">
+  <autoFilter ref="A1:G85">
     <filterColumn colId="4">
       <filters>
-        <filter val="Toma"/>
+        <filter val="Daniel"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Tasks update, tutorial level and level 01 done
</commit_message>
<xml_diff>
--- a/SAWZE_Documentation/Last Mile/SAWZE_priority_plan.xlsx
+++ b/SAWZE_Documentation/Last Mile/SAWZE_priority_plan.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tabelle2!$A$1:$G$85</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tabelle2!$A$1:$G$86</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="156">
   <si>
     <t>Gameplay</t>
   </si>
@@ -261,9 +261,6 @@
     <t>slow_Boden</t>
   </si>
   <si>
-    <t>optimize, center</t>
-  </si>
-  <si>
     <t>game over</t>
   </si>
   <si>
@@ -330,9 +327,6 @@
     <t>Alarm</t>
   </si>
   <si>
-    <t>Script (trigger, effekt, zombie pathfind.,hero, zombie turn)</t>
-  </si>
-  <si>
     <t>Comic Cloud</t>
   </si>
   <si>
@@ -466,6 +460,33 @@
   </si>
   <si>
     <t>balancing of Healt loss out of the cloud</t>
+  </si>
+  <si>
+    <t>Vignett polieren</t>
+  </si>
+  <si>
+    <t>optimize, center, - TAKE OFF (?)</t>
+  </si>
+  <si>
+    <t>xxx</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Controller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">einbauen </t>
+  </si>
+  <si>
+    <t>Script  (trigger, effekt, zombie pathfind)</t>
+  </si>
+  <si>
+    <t>Script (hero - strong, fast, zombie turn, timer, )</t>
+  </si>
+  <si>
+    <t>Script (und etwas modell hero vibriert, shaked, weis halt was ich mein, gell)</t>
   </si>
 </sst>
 </file>
@@ -559,7 +580,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -579,6 +600,12 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1127,11 +1154,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:G85"/>
+  <dimension ref="A1:G87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F85" sqref="F85"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D87" sqref="D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1139,7 +1166,7 @@
     <col min="1" max="1" width="12.140625" style="4" customWidth="1"/>
     <col min="2" max="2" width="15" style="4" customWidth="1"/>
     <col min="3" max="3" width="8.140625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" style="12" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" style="4"/>
     <col min="6" max="6" width="81.42578125" style="4" customWidth="1"/>
   </cols>
@@ -1154,7 +1181,7 @@
       <c r="C1" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>44</v>
       </c>
       <c r="E1" s="8" t="s">
@@ -1164,12 +1191,12 @@
         <v>46</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>12</v>
@@ -1179,15 +1206,15 @@
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>12</v>
@@ -1197,25 +1224,25 @@
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>38</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1228,7 +1255,7 @@
       <c r="C5" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="5"/>
+      <c r="D5" s="13"/>
       <c r="E5" s="4" t="s">
         <v>47</v>
       </c>
@@ -1246,12 +1273,15 @@
       <c r="C6" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="5"/>
+      <c r="D6" s="13"/>
       <c r="E6" s="4" t="s">
         <v>47</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>73</v>
+      </c>
+      <c r="G6" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1264,7 +1294,7 @@
       <c r="C7" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="5"/>
+      <c r="D7" s="13"/>
       <c r="E7" s="4" t="s">
         <v>47</v>
       </c>
@@ -1295,7 +1325,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>38</v>
@@ -1305,7 +1335,7 @@
         <v>54</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1313,17 +1343,20 @@
         <v>2</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="5"/>
+      <c r="D10" s="13"/>
       <c r="E10" s="4" t="s">
         <v>47</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>60</v>
+      </c>
+      <c r="G10" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1331,7 +1364,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>38</v>
@@ -1341,7 +1374,7 @@
         <v>54</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1349,17 +1382,20 @@
         <v>2</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="5"/>
+      <c r="D12" s="13"/>
       <c r="E12" s="4" t="s">
         <v>47</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>60</v>
+      </c>
+      <c r="G12" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1367,20 +1403,20 @@
         <v>2</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>88</v>
-      </c>
       <c r="G13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1388,7 +1424,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>38</v>
@@ -1398,7 +1434,7 @@
         <v>54</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1406,20 +1442,20 @@
         <v>2</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="13"/>
+      <c r="E15" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C15" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>93</v>
-      </c>
       <c r="G15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1427,17 +1463,17 @@
         <v>2</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="13"/>
+      <c r="E16" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>94</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1445,20 +1481,20 @@
         <v>2</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="5"/>
+      <c r="D17" s="13"/>
       <c r="E17" s="4" t="s">
         <v>47</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1466,7 +1502,7 @@
         <v>2</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>39</v>
@@ -1476,7 +1512,7 @@
         <v>54</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1484,7 +1520,7 @@
         <v>2</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>38</v>
@@ -1494,10 +1530,10 @@
         <v>67</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1510,7 +1546,7 @@
       <c r="C20" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="5"/>
+      <c r="D20" s="13"/>
       <c r="E20" s="4" t="s">
         <v>47</v>
       </c>
@@ -1523,12 +1559,12 @@
         <v>0</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="5"/>
+      <c r="D21" s="13"/>
       <c r="E21" s="4" t="s">
         <v>47</v>
       </c>
@@ -1536,7 +1572,7 @@
         <v>49</v>
       </c>
       <c r="G21" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1575,7 +1611,7 @@
         <v>56</v>
       </c>
       <c r="G23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1623,14 +1659,16 @@
         <v>58</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D26" s="5"/>
+        <v>149</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>150</v>
+      </c>
       <c r="E26" s="4" t="s">
         <v>47</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>80</v>
+        <v>148</v>
       </c>
       <c r="G26" s="6"/>
     </row>
@@ -1644,7 +1682,7 @@
       <c r="C27" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D27" s="5"/>
+      <c r="D27" s="14"/>
       <c r="E27" s="4" t="s">
         <v>47</v>
       </c>
@@ -1693,12 +1731,12 @@
         <v>50</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C30" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="5"/>
+      <c r="D30" s="13"/>
       <c r="E30" s="4" t="s">
         <v>47</v>
       </c>
@@ -1711,7 +1749,7 @@
         <v>50</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C31" s="12" t="s">
         <v>38</v>
@@ -1729,7 +1767,7 @@
         <v>50</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C32" s="12" t="s">
         <v>38</v>
@@ -1739,7 +1777,7 @@
         <v>55</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1757,7 +1795,7 @@
         <v>67</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1765,7 +1803,7 @@
         <v>50</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C34" s="12" t="s">
         <v>38</v>
@@ -1775,7 +1813,7 @@
         <v>67</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1783,7 +1821,7 @@
         <v>50</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C35" s="12" t="s">
         <v>38</v>
@@ -1793,7 +1831,7 @@
         <v>67</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1801,7 +1839,7 @@
         <v>70</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C36" s="12" t="s">
         <v>38</v>
@@ -1811,7 +1849,7 @@
         <v>55</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1819,17 +1857,17 @@
         <v>70</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C37" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D37" s="5"/>
+      <c r="D37" s="13"/>
       <c r="E37" s="4" t="s">
         <v>47</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>60</v>
+        <v>153</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1837,12 +1875,12 @@
         <v>70</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C38" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D38" s="5"/>
+      <c r="D38" s="13"/>
       <c r="E38" s="4" t="s">
         <v>47</v>
       </c>
@@ -1850,7 +1888,7 @@
         <v>1</v>
       </c>
       <c r="G38" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1858,7 +1896,7 @@
         <v>70</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C39" s="12" t="s">
         <v>38</v>
@@ -1876,17 +1914,17 @@
         <v>70</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C40" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D40" s="5"/>
+      <c r="D40" s="13"/>
       <c r="E40" s="4" t="s">
         <v>47</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>103</v>
+        <v>154</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -1894,12 +1932,12 @@
         <v>70</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C41" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D41" s="5"/>
+      <c r="D41" s="13"/>
       <c r="E41" s="4" t="s">
         <v>47</v>
       </c>
@@ -1907,7 +1945,7 @@
         <v>1</v>
       </c>
       <c r="G41" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1915,14 +1953,14 @@
         <v>7</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C42" s="12" t="s">
         <v>38</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1930,14 +1968,14 @@
         <v>7</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C43" s="12" t="s">
         <v>38</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F43" s="4" t="s">
         <v>29</v>
@@ -1948,14 +1986,14 @@
         <v>7</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C44" s="12" t="s">
         <v>38</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1963,14 +2001,14 @@
         <v>7</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C45" s="12" t="s">
         <v>38</v>
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1978,14 +2016,14 @@
         <v>7</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C46" s="12" t="s">
         <v>39</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1993,17 +2031,17 @@
         <v>7</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C47" s="12" t="s">
         <v>38</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G47" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -2011,14 +2049,14 @@
         <v>7</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C48" s="12" t="s">
         <v>38</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -2026,97 +2064,97 @@
         <v>7</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C49" s="12" t="s">
         <v>39</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D50" s="13"/>
+      <c r="E50" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F50" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C50" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D50" s="5"/>
-      <c r="E50" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F50" s="4" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C51" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D51" s="5"/>
+      <c r="D51" s="13"/>
       <c r="E51" s="4" t="s">
         <v>47</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G51" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C52" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D52" s="5"/>
+      <c r="D52" s="13"/>
       <c r="E52" s="4" t="s">
         <v>47</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B53" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D53" s="13"/>
+      <c r="E53" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F53" s="4" t="s">
         <v>120</v>
-      </c>
-      <c r="C53" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D53" s="5"/>
-      <c r="E53" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F53" s="4" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C54" s="12" t="s">
         <v>38</v>
@@ -2126,15 +2164,15 @@
         <v>54</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C55" s="12" t="s">
         <v>39</v>
@@ -2144,7 +2182,7 @@
         <v>67</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -2175,12 +2213,12 @@
       <c r="C57" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D57" s="5"/>
+      <c r="D57" s="13"/>
       <c r="E57" s="4" t="s">
         <v>47</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -2211,7 +2249,7 @@
       <c r="C59" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D59" s="5"/>
+      <c r="D59" s="13"/>
       <c r="E59" s="4" t="s">
         <v>47</v>
       </c>
@@ -2247,7 +2285,7 @@
       <c r="C61" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D61" s="5"/>
+      <c r="D61" s="13"/>
       <c r="E61" s="4" t="s">
         <v>47</v>
       </c>
@@ -2283,12 +2321,12 @@
       <c r="C63" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D63" s="5"/>
+      <c r="D63" s="13"/>
       <c r="E63" s="4" t="s">
         <v>47</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -2319,12 +2357,12 @@
       <c r="C65" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D65" s="5"/>
+      <c r="D65" s="13"/>
       <c r="E65" s="4" t="s">
         <v>47</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -2353,14 +2391,14 @@
         <v>68</v>
       </c>
       <c r="C67" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D67" s="5"/>
+        <v>38</v>
+      </c>
+      <c r="D67" s="13"/>
       <c r="E67" s="4" t="s">
         <v>47</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -2371,17 +2409,17 @@
         <v>68</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D68" s="5"/>
+        <v>38</v>
+      </c>
+      <c r="D68" s="13"/>
       <c r="E68" s="4" t="s">
         <v>47</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G68" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -2466,12 +2504,12 @@
       <c r="C73" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D73" s="5"/>
+      <c r="D73" s="13"/>
       <c r="E73" s="4" t="s">
         <v>47</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>60</v>
+        <v>155</v>
       </c>
     </row>
     <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -2479,7 +2517,7 @@
         <v>77</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C74" s="12" t="s">
         <v>38</v>
@@ -2489,7 +2527,7 @@
         <v>55</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -2497,7 +2535,7 @@
         <v>77</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C75" s="12" t="s">
         <v>38</v>
@@ -2512,7 +2550,7 @@
         <v>77</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C76" s="12" t="s">
         <v>38</v>
@@ -2532,17 +2570,17 @@
       <c r="C77" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D77" s="5"/>
+      <c r="D77" s="13"/>
       <c r="E77" s="4" t="s">
         <v>47</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B78" s="4" t="s">
         <v>5</v>
@@ -2552,40 +2590,40 @@
       </c>
       <c r="D78" s="5"/>
       <c r="E78" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C79" s="12" t="s">
         <v>38</v>
       </c>
       <c r="D79" s="5"/>
       <c r="E79" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C80" s="12" t="s">
         <v>38</v>
       </c>
       <c r="D80" s="5"/>
       <c r="E80" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -2593,38 +2631,38 @@
         <v>0</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C81" s="12" t="s">
         <v>38</v>
       </c>
       <c r="D81" s="5"/>
       <c r="E81" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C82" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D82" s="5"/>
+      <c r="D82" s="13"/>
       <c r="E82" s="4" t="s">
         <v>47</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G82" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -2632,17 +2670,17 @@
         <v>0</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C83" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D83" s="5"/>
+      <c r="D83" s="13"/>
       <c r="E83" s="4" t="s">
         <v>47</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -2650,7 +2688,7 @@
         <v>61</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C84" s="12" t="s">
         <v>38</v>
@@ -2660,7 +2698,7 @@
         <v>67</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="85" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -2668,21 +2706,57 @@
         <v>0</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C85" s="12" t="s">
         <v>38</v>
       </c>
       <c r="D85" s="5"/>
       <c r="E85" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C86" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D86" s="5"/>
+      <c r="E86" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F86" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C87" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D87" s="13"/>
+      <c r="E87" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F87" s="4" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G85">
+  <autoFilter ref="A1:G86">
     <filterColumn colId="4">
       <filters>
         <filter val="Daniel"/>
@@ -2690,6 +2764,7 @@
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Level 1,2,3,4, update, Task sheet update
</commit_message>
<xml_diff>
--- a/SAWZE_Documentation/Last Mile/SAWZE_priority_plan.xlsx
+++ b/SAWZE_Documentation/Last Mile/SAWZE_priority_plan.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tabelle2!$A$1:$G$86</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tabelle2!$A$1:$G$84</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="161">
   <si>
     <t>Gameplay</t>
   </si>
@@ -387,12 +387,6 @@
     <t>animation</t>
   </si>
   <si>
-    <t>TS icon</t>
-  </si>
-  <si>
-    <t>Kopf der verschiedenen TSs als Icon in GUI</t>
-  </si>
-  <si>
     <t>Text box</t>
   </si>
   <si>
@@ -411,12 +405,6 @@
     <t>sound ?</t>
   </si>
   <si>
-    <t>Sad Hero (only Face)</t>
-  </si>
-  <si>
-    <t>happy Hero (only Face)</t>
-  </si>
-  <si>
     <t>zombie chase hero, animation for the main menu</t>
   </si>
   <si>
@@ -487,13 +475,40 @@
   </si>
   <si>
     <t>Script (und etwas modell hero vibriert, shaked, weis halt was ich mein, gell)</t>
+  </si>
+  <si>
+    <t>Sad Hero (only Face) Highpoly</t>
+  </si>
+  <si>
+    <t>happy Hero (only Face) Highpoly</t>
+  </si>
+  <si>
+    <t>new partkel effekt</t>
+  </si>
+  <si>
+    <t>Gamer</t>
+  </si>
+  <si>
+    <t>unic lvl assets_2</t>
+  </si>
+  <si>
+    <t>unic lvl assets_1</t>
+  </si>
+  <si>
+    <t>Level 02</t>
+  </si>
+  <si>
+    <t>Level 03</t>
+  </si>
+  <si>
+    <t>Level 04</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -509,8 +524,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -538,6 +560,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -580,7 +608,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -606,6 +634,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1153,12 +1185,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:G87"/>
+  <dimension ref="A1:G84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D87" sqref="D87"/>
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1194,7 +1225,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>107</v>
       </c>
@@ -1209,10 +1240,10 @@
         <v>105</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>107</v>
       </c>
@@ -1227,7 +1258,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>107</v>
       </c>
@@ -1255,7 +1286,7 @@
       <c r="C5" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="13"/>
+      <c r="D5" s="14"/>
       <c r="E5" s="4" t="s">
         <v>47</v>
       </c>
@@ -1302,7 +1333,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>2</v>
       </c>
@@ -1312,7 +1343,7 @@
       <c r="C8" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="5"/>
+      <c r="D8" s="7"/>
       <c r="E8" s="4" t="s">
         <v>67</v>
       </c>
@@ -1320,7 +1351,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>2</v>
       </c>
@@ -1359,7 +1390,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>2</v>
       </c>
@@ -1419,7 +1450,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>2</v>
       </c>
@@ -1429,7 +1460,7 @@
       <c r="C14" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="5"/>
+      <c r="D14" s="15"/>
       <c r="E14" s="4" t="s">
         <v>54</v>
       </c>
@@ -1468,7 +1499,7 @@
       <c r="C16" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="13"/>
+      <c r="D16" s="14"/>
       <c r="E16" s="4" t="s">
         <v>47</v>
       </c>
@@ -1497,7 +1528,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>2</v>
       </c>
@@ -1507,20 +1538,20 @@
       <c r="C18" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="5"/>
+      <c r="D18" s="15"/>
       <c r="E18" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>38</v>
@@ -1530,7 +1561,7 @@
         <v>67</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G19" t="s">
         <v>84</v>
@@ -1564,7 +1595,7 @@
       <c r="C21" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="13"/>
+      <c r="D21" s="14"/>
       <c r="E21" s="4" t="s">
         <v>47</v>
       </c>
@@ -1572,10 +1603,10 @@
         <v>49</v>
       </c>
       <c r="G21" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>50</v>
       </c>
@@ -1585,7 +1616,7 @@
       <c r="C22" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="5"/>
+      <c r="D22" s="15"/>
       <c r="E22" s="4" t="s">
         <v>54</v>
       </c>
@@ -1593,62 +1624,62 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>50</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D23" s="5"/>
+      <c r="D23" s="15"/>
       <c r="E23" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="G23" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="G23" s="6"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>50</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" s="5"/>
+        <v>145</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>146</v>
+      </c>
       <c r="E24" s="4" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>53</v>
+        <v>144</v>
       </c>
       <c r="G24" s="6"/>
     </row>
-    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>50</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C25" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="5"/>
+      <c r="D25" s="14"/>
       <c r="E25" s="4" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1656,21 +1687,18 @@
         <v>50</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>150</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="D26" s="15"/>
       <c r="E26" s="4" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="G26" s="6"/>
+        <v>53</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
@@ -1682,48 +1710,48 @@
       <c r="C27" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D27" s="14"/>
+      <c r="D27" s="7"/>
       <c r="E27" s="4" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>50</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="C28" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D28" s="5"/>
+      <c r="D28" s="14"/>
       <c r="E28" s="4" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>50</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="C29" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D29" s="5"/>
+      <c r="D29" s="15"/>
       <c r="E29" s="4" t="s">
         <v>55</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1736,110 +1764,113 @@
       <c r="C30" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="13"/>
+      <c r="D30" s="7"/>
       <c r="E30" s="4" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>50</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>89</v>
+        <v>19</v>
       </c>
       <c r="C31" s="12" t="s">
         <v>38</v>
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="4" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>50</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C32" s="12" t="s">
         <v>38</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33" s="7"/>
+      <c r="E33" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F32" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D33" s="5"/>
-      <c r="E33" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="F33" s="4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>82</v>
+        <v>101</v>
       </c>
       <c r="C34" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D34" s="5"/>
+      <c r="D34" s="14"/>
       <c r="E34" s="4" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="C35" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D35" s="5"/>
+      <c r="D35" s="13"/>
       <c r="E35" s="4" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="G35" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>70</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C36" s="12" t="s">
         <v>38</v>
@@ -1849,7 +1880,7 @@
         <v>55</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1857,17 +1888,17 @@
         <v>70</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C37" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D37" s="13"/>
+      <c r="D37" s="14"/>
       <c r="E37" s="4" t="s">
         <v>47</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1875,7 +1906,7 @@
         <v>70</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C38" s="12" t="s">
         <v>38</v>
@@ -1891,97 +1922,85 @@
         <v>84</v>
       </c>
     </row>
-    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="C39" s="12" t="s">
         <v>38</v>
       </c>
       <c r="D39" s="5"/>
       <c r="E39" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>52</v>
+        <v>105</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="C40" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D40" s="13"/>
+      <c r="D40" s="7"/>
       <c r="E40" s="4" t="s">
-        <v>47</v>
+        <v>106</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>154</v>
+        <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>99</v>
+        <v>158</v>
       </c>
       <c r="C41" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D41" s="13"/>
+      <c r="D41" s="5"/>
       <c r="E41" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G41" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>104</v>
+        <v>159</v>
       </c>
       <c r="C42" s="12" t="s">
         <v>38</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>104</v>
+        <v>160</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="F43" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>7</v>
       </c>
@@ -1993,10 +2012,13 @@
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="G44" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>7</v>
       </c>
@@ -2008,10 +2030,10 @@
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>7</v>
       </c>
@@ -2023,63 +2045,72 @@
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>7</v>
+        <v>111</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C47" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D47" s="5"/>
+      <c r="D47" s="13"/>
       <c r="E47" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="G47" t="s">
+        <v>47</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D48" s="13"/>
+      <c r="E48" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="G48" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C48" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D48" s="5"/>
-      <c r="E48" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>7</v>
+        <v>111</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D49" s="5"/>
+        <v>38</v>
+      </c>
+      <c r="D49" s="13"/>
       <c r="E49" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>111</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="C50" s="12" t="s">
         <v>38</v>
@@ -2089,262 +2120,259 @@
         <v>47</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>111</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="C51" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D51" s="13"/>
+      <c r="D51" s="5"/>
       <c r="E51" s="4" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="G51" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>111</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D52" s="13"/>
+        <v>39</v>
+      </c>
+      <c r="D52" s="5"/>
       <c r="E52" s="4" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>111</v>
+        <v>61</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>118</v>
+        <v>62</v>
       </c>
       <c r="C53" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D53" s="13"/>
+      <c r="D53" s="7"/>
       <c r="E53" s="4" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>111</v>
+        <v>61</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>119</v>
+        <v>62</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D54" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="D54" s="13"/>
       <c r="E54" s="4" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>111</v>
+        <v>61</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>121</v>
+        <v>63</v>
       </c>
       <c r="C55" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D55" s="5"/>
+      <c r="D55" s="7"/>
       <c r="E55" s="4" t="s">
         <v>67</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>61</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D56" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="D56" s="13"/>
       <c r="E56" s="4" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>61</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D57" s="13"/>
+        <v>38</v>
+      </c>
+      <c r="D57" s="7"/>
       <c r="E57" s="4" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>61</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C58" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D58" s="5"/>
+      <c r="D58" s="13"/>
       <c r="E58" s="4" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>61</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C59" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D59" s="13"/>
+      <c r="D59" s="5"/>
       <c r="E59" s="4" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>61</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D60" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="D60" s="13"/>
       <c r="E60" s="4" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>61</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C61" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D61" s="13"/>
+      <c r="D61" s="5"/>
       <c r="E61" s="4" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>61</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C62" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D62" s="5"/>
+      <c r="D62" s="13"/>
       <c r="E62" s="4" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>61</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D63" s="13"/>
+        <v>38</v>
+      </c>
+      <c r="D63" s="7"/>
       <c r="E63" s="4" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>61</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D64" s="5"/>
+        <v>38</v>
+      </c>
+      <c r="D64" s="14"/>
       <c r="E64" s="4" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -2352,118 +2380,115 @@
         <v>61</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D65" s="13"/>
       <c r="E65" s="4" t="s">
         <v>47</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="C66" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D66" s="5"/>
+      <c r="D66" s="7"/>
       <c r="E66" s="4" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="C67" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D67" s="13"/>
+      <c r="D67" s="7"/>
       <c r="E67" s="4" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>87</v>
+        <v>52</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="C68" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D68" s="13"/>
+      <c r="D68" s="14"/>
       <c r="E68" s="4" t="s">
         <v>47</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="G68" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>77</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="C69" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D69" s="5"/>
+      <c r="D69" s="7"/>
       <c r="E69" s="4" t="s">
         <v>55</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>77</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>78</v>
+        <v>157</v>
       </c>
       <c r="C70" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D70" s="5"/>
+      <c r="D70" s="15"/>
       <c r="E70" s="4" t="s">
         <v>54</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>77</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>79</v>
+        <v>125</v>
       </c>
       <c r="C71" s="12" t="s">
         <v>38</v>
@@ -2472,100 +2497,97 @@
       <c r="E71" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F71" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>77</v>
+        <v>7</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>79</v>
+        <v>29</v>
       </c>
       <c r="C72" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D72" s="5"/>
+      <c r="D72" s="13"/>
       <c r="E72" s="4" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>52</v>
+        <v>129</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>77</v>
+        <v>107</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>79</v>
+        <v>5</v>
       </c>
       <c r="C73" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D73" s="13"/>
+      <c r="D73" s="5"/>
       <c r="E73" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F73" s="4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>77</v>
+        <v>107</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>96</v>
+        <v>130</v>
       </c>
       <c r="C74" s="12" t="s">
         <v>38</v>
       </c>
       <c r="D74" s="7"/>
       <c r="E74" s="4" t="s">
-        <v>55</v>
+        <v>106</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>77</v>
+        <v>107</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="C75" s="12" t="s">
         <v>38</v>
       </c>
       <c r="D75" s="5"/>
       <c r="E75" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="C76" s="12" t="s">
         <v>38</v>
       </c>
       <c r="D76" s="5"/>
       <c r="E76" s="4" t="s">
-        <v>55</v>
+        <v>106</v>
+      </c>
+      <c r="F76" s="4" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>7</v>
+        <v>111</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>29</v>
+        <v>135</v>
       </c>
       <c r="C77" s="12" t="s">
         <v>38</v>
@@ -2575,48 +2597,54 @@
         <v>47</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="G77" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>107</v>
+        <v>0</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>5</v>
+        <v>137</v>
       </c>
       <c r="C78" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D78" s="5"/>
+      <c r="D78" s="14"/>
       <c r="E78" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>107</v>
+        <v>61</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="C79" s="12" t="s">
         <v>38</v>
       </c>
       <c r="D79" s="5"/>
       <c r="E79" s="4" t="s">
-        <v>106</v>
+        <v>67</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>107</v>
+        <v>0</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C80" s="12" t="s">
         <v>38</v>
@@ -2625,31 +2653,34 @@
       <c r="E80" s="4" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F80" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C81" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D81" s="7"/>
+      <c r="E81" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F81" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B81" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="C81" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D81" s="5"/>
-      <c r="E81" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="F81" s="4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="4" t="s">
-        <v>111</v>
-      </c>
       <c r="B82" s="4" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="C82" s="12" t="s">
         <v>38</v>
@@ -2659,110 +2690,47 @@
         <v>47</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="G82" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>141</v>
+        <v>91</v>
       </c>
       <c r="C83" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D83" s="13"/>
+      <c r="D83" s="5"/>
       <c r="E83" s="4" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>144</v>
+        <v>156</v>
       </c>
       <c r="C84" s="12" t="s">
         <v>38</v>
       </c>
       <c r="D84" s="5"/>
       <c r="E84" s="4" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B85" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C85" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D85" s="5"/>
-      <c r="E85" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="F85" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B86" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C86" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D86" s="5"/>
-      <c r="E86" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F86" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B87" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="C87" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D87" s="13"/>
-      <c r="E87" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F87" s="4" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G86">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="Daniel"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:G84"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>